<commit_message>
Ajustements divers liés à la correction de l'outil cross-validateur DRIM-M Ajout d'un onglet permettant le mapping entre les jeux de données référencement et les scénarios de test associés
</commit_message>
<xml_diff>
--- a/Référencement DRIMBox/Récapitulatif jeux de données/Matrice usage jeux de données.xlsx
+++ b/Référencement DRIMBox/Récapitulatif jeux de données/Matrice usage jeux de données.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Partage\ald\Projet DIM\Dataset\Récap Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Desktop\GIT DRIM\GIT ANS\DRIM-M_DATA\Référencement DRIMBox\Récapitulatif jeux de données\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDACE3DB-7C50-40A8-9358-5CC4CB387B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7717E183-9FE6-4274-8DA0-30A872D6B293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="888" activeTab="2" xr2:uid="{BB8B18FC-8678-491B-A674-F261D34D6FC9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="888" xr2:uid="{BB8B18FC-8678-491B-A674-F261D34D6FC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Usage_IMG" sheetId="31" r:id="rId1"/>
-    <sheet name="Usage_CR" sheetId="32" r:id="rId2"/>
-    <sheet name="Usage_KOS" sheetId="33" r:id="rId3"/>
+    <sheet name="Mapping dataset_scénarios" sheetId="34" r:id="rId1"/>
+    <sheet name="Usage_IMG" sheetId="31" r:id="rId2"/>
+    <sheet name="Usage_CR" sheetId="32" r:id="rId3"/>
+    <sheet name="Usage_KOS" sheetId="33" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Usage_CR!$A$1:$H$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Usage_IMG!$A$1:$F$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Usage_KOS!$A$1:$F$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Usage_CR!$A$1:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Usage_IMG!$A$1:$F$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Usage_KOS!$A$1:$F$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="191">
   <si>
     <t xml:space="preserve">Jeu de données </t>
   </si>
@@ -451,13 +452,178 @@
   </si>
   <si>
     <t>* Une publication du KOS pourra avoir lieu si l'éditeur choisit d'interagir avec le DMP sans que le cas de test ne l'impose</t>
+  </si>
+  <si>
+    <t>Examen A</t>
+  </si>
+  <si>
+    <t>Examen B</t>
+  </si>
+  <si>
+    <t>Examen C</t>
+  </si>
+  <si>
+    <t>Examen D</t>
+  </si>
+  <si>
+    <t>Examen E</t>
+  </si>
+  <si>
+    <t>Examen F1</t>
+  </si>
+  <si>
+    <t>Examen F2</t>
+  </si>
+  <si>
+    <t>Examen G</t>
+  </si>
+  <si>
+    <t>Examen H</t>
+  </si>
+  <si>
+    <t>Examen I</t>
+  </si>
+  <si>
+    <t>Examen J</t>
+  </si>
+  <si>
+    <t>Examen K</t>
+  </si>
+  <si>
+    <t>Examen L</t>
+  </si>
+  <si>
+    <t>Examen M</t>
+  </si>
+  <si>
+    <t>Examen N</t>
+  </si>
+  <si>
+    <t>Examen O</t>
+  </si>
+  <si>
+    <t>Examen P</t>
+  </si>
+  <si>
+    <t>Examen Q</t>
+  </si>
+  <si>
+    <t>Examen R</t>
+  </si>
+  <si>
+    <t>Examen S</t>
+  </si>
+  <si>
+    <t>Examen T</t>
+  </si>
+  <si>
+    <t>Examen U</t>
+  </si>
+  <si>
+    <t>Examen V</t>
+  </si>
+  <si>
+    <t>Examen W</t>
+  </si>
+  <si>
+    <t>Examen X</t>
+  </si>
+  <si>
+    <t>Examen Y</t>
+  </si>
+  <si>
+    <t>Examen Z</t>
+  </si>
+  <si>
+    <t>Examen de référence</t>
+  </si>
+  <si>
+    <t>Cas de test associé</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_CONSO_IMG.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_REPONSE_WADO.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_APPEL_CONTEXTUEL.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_EXPORT.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_PRODUCTION.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_PROXY_INTERACTION_PACS</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_ARCHIVE_KOS.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_PROXY_MULTI_RIS_PACS.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_NATIF_MULTI_RIS.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_CONVERSION.01 (DB.SO.41.01)</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_SERIALISATION.01 (DB.CO.122.01)</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_WADO_ERR.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_mTLS.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_mTLS.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_APPEL_URL.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_RESYNCHRONISATION.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_PROXY_IOCM.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_FRANCE_CONNECT.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_CONSULTATION_CR.01 (DB.CO.58.01)</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_RECUPERATION_KOS.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_CO_PERFORMANCE.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_PROXY_PERFORMANCE.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_NATIF_PERFORMANCE.01</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_Proxy_HL7v2OMI.01 (DB.SO.133.01)</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_NATIF_MAJ_KOS.01 (DB.SO.27.01)</t>
+  </si>
+  <si>
+    <t>DRIM-M_SO_PROXY_CONNEXION_PACS.01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +647,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -490,7 +664,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -756,11 +930,215 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -855,6 +1233,70 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,11 +1611,353 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1F3031-10C5-4AC1-B014-6D9F1C0FB6B7}">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="44"/>
+      <c r="B6" s="53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="48"/>
+      <c r="B12" s="55" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="48"/>
+      <c r="B17" s="55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="48"/>
+      <c r="B23" s="57" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="48"/>
+      <c r="B26" s="57" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="44"/>
+      <c r="B29" s="53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="48"/>
+      <c r="B30" s="55" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="44"/>
+      <c r="B32" s="58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="44"/>
+      <c r="B33" s="58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="44"/>
+      <c r="B34" s="53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="44"/>
+      <c r="B35" s="53" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="48"/>
+      <c r="B36" s="55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="51" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="51" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" s="54" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="48"/>
+      <c r="B40" s="57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" s="56" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" s="62" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A28:A30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC27A141-FE22-485A-AF20-DC6FC6F943BA}">
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -1986,7 +2770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA04F3FB-916B-4A27-89B7-53B8024D583C}">
   <dimension ref="A1:H34"/>
   <sheetViews>
@@ -2835,11 +3619,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F9E2D9-76DB-4EDC-8C79-9E43E7831D2D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>

</xml_diff>